<commit_message>
added expense and income
</commit_message>
<xml_diff>
--- a/server/Expenses.xlsx
+++ b/server/Expenses.xlsx
@@ -404,29 +404,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="C1" t="str">
         <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Source</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Amount</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Food</v>
+      </c>
+      <c r="B2">
+        <v>3000</v>
+      </c>
+      <c r="C2" t="str">
         <v>2025-07-21</v>
-      </c>
-      <c r="C2">
-        <v>3000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>Food</v>
+      </c>
+      <c r="B3">
+        <v>3000</v>
+      </c>
+      <c r="C3" t="str">
         <v>2025-07-21</v>
-      </c>
-      <c r="C3">
-        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>